<commit_message>
banging my head against the wall with tidyeval
</commit_message>
<xml_diff>
--- a/educ_cats.xlsx
+++ b/educ_cats.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\User\Williams\Data Assistance\mnmigration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\User\Williams\Data\mnmigration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="8880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="8880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>N/A or no schooling</t>
   </si>
@@ -186,19 +187,34 @@
   </si>
   <si>
     <t>Some College, No Degree</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>IPUMS CAT</t>
+  </si>
+  <si>
+    <t>My Category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,8 +237,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1011,5 +1033,357 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>N/A</v>
+      </c>
+      <c r="C2" t="str">
+        <f>VLOOKUP(A2, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>NA/Missing</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>No schooling completed</v>
+      </c>
+      <c r="C3" t="str">
+        <f>VLOOKUP(A3, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>11</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Nursery school, preschool</v>
+      </c>
+      <c r="C4" t="str">
+        <f>VLOOKUP(A4, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>12</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Kindergarten</v>
+      </c>
+      <c r="C5" t="str">
+        <f>VLOOKUP(A5, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>14</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 1</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP(A6, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>15</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 2</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(A7, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>16</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 3</v>
+      </c>
+      <c r="C8" t="str">
+        <f>VLOOKUP(A8, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>17</v>
+      </c>
+      <c r="B9" t="str">
+        <f>VLOOKUP(A9, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 4</v>
+      </c>
+      <c r="C9" t="str">
+        <f>VLOOKUP(A9, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>22</v>
+      </c>
+      <c r="B10" t="str">
+        <f>VLOOKUP(A10, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 5</v>
+      </c>
+      <c r="C10" t="str">
+        <f>VLOOKUP(A10, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>23</v>
+      </c>
+      <c r="B11" t="str">
+        <f>VLOOKUP(A11, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 6</v>
+      </c>
+      <c r="C11" t="str">
+        <f>VLOOKUP(A11, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>25</v>
+      </c>
+      <c r="B12" t="str">
+        <f>VLOOKUP(A12, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 7</v>
+      </c>
+      <c r="C12" t="str">
+        <f>VLOOKUP(A12, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>26</v>
+      </c>
+      <c r="B13" t="str">
+        <f>VLOOKUP(A13, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 8</v>
+      </c>
+      <c r="C13" t="str">
+        <f>VLOOKUP(A13, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>30</v>
+      </c>
+      <c r="B14" t="str">
+        <f>VLOOKUP(A14, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 9</v>
+      </c>
+      <c r="C14" t="str">
+        <f>VLOOKUP(A14, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>40</v>
+      </c>
+      <c r="B15" t="str">
+        <f>VLOOKUP(A15, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 10</v>
+      </c>
+      <c r="C15" t="str">
+        <f>VLOOKUP(A15, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>50</v>
+      </c>
+      <c r="B16" t="str">
+        <f>VLOOKUP(A16, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Grade 11</v>
+      </c>
+      <c r="C16" t="str">
+        <f>VLOOKUP(A16, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>61</v>
+      </c>
+      <c r="B17" t="str">
+        <f>VLOOKUP(A17, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>12th grade, no diploma</v>
+      </c>
+      <c r="C17" t="str">
+        <f>VLOOKUP(A17, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Less than HS Diploma</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>63</v>
+      </c>
+      <c r="B18" t="str">
+        <f>VLOOKUP(A18, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Regular high school diploma</v>
+      </c>
+      <c r="C18" t="str">
+        <f>VLOOKUP(A18, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>High School/GED</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>64</v>
+      </c>
+      <c r="B19" t="str">
+        <f>VLOOKUP(A19, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>GED or alternative credential</v>
+      </c>
+      <c r="C19" t="str">
+        <f>VLOOKUP(A19, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>High School/GED</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>65</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP(A20, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Some college, but less than 1 year</v>
+      </c>
+      <c r="C20" t="str">
+        <f>VLOOKUP(A20, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Some College, No Degree</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>71</v>
+      </c>
+      <c r="B21" t="str">
+        <f>VLOOKUP(A21, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>1 or more years of college credit, no degree</v>
+      </c>
+      <c r="C21" t="str">
+        <f>VLOOKUP(A21, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Some College, No Degree</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>81</v>
+      </c>
+      <c r="B22" t="str">
+        <f>VLOOKUP(A22, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Associate's degree, type not specified</v>
+      </c>
+      <c r="C22" t="str">
+        <f>VLOOKUP(A22, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Associate's Degree</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>101</v>
+      </c>
+      <c r="B23" t="str">
+        <f>VLOOKUP(A23, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Bachelor's degree</v>
+      </c>
+      <c r="C23" t="str">
+        <f>VLOOKUP(A23, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Bachelor's Degree</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>114</v>
+      </c>
+      <c r="B24" t="str">
+        <f>VLOOKUP(A24, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Master's degree</v>
+      </c>
+      <c r="C24" t="str">
+        <f>VLOOKUP(A24, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Advanced Degree</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>115</v>
+      </c>
+      <c r="B25" t="str">
+        <f>VLOOKUP(A25, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Professional degree beyond a bachelor's degree</v>
+      </c>
+      <c r="C25" t="str">
+        <f>VLOOKUP(A25, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Advanced Degree</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>116</v>
+      </c>
+      <c r="B26" t="str">
+        <f>VLOOKUP(A26, Sheet1!$A$2:$C$45, 2, FALSE)</f>
+        <v>Doctoral degree</v>
+      </c>
+      <c r="C26" t="str">
+        <f>VLOOKUP(A26, Sheet1!$A$2:$C$45, 3, FALSE)</f>
+        <v>Advanced Degree</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>